<commit_message>
Populated the Phase 1 Frequency Database
</commit_message>
<xml_diff>
--- a/book/DATA/phase1_frequency_matrix_populated.xlsx
+++ b/book/DATA/phase1_frequency_matrix_populated.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\aimoralcode-core\book\DATA\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0604FCDD-B8BA-4725-B166-D3D5D3F3380A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -2990,8 +2996,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3067,13 +3073,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3111,7 +3125,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -3145,6 +3159,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -3179,9 +3194,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3354,14 +3370,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W292"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A256" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="19" max="19" width="121.21875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="171" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="31.88671875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="29.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3432,7 +3454,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -3497,7 +3519,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -3562,7 +3584,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -3627,7 +3649,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="5" spans="1:23">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -3692,7 +3714,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="6" spans="1:23">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -3757,7 +3779,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="7" spans="1:23">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -3822,7 +3844,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="8" spans="1:23">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -3887,7 +3909,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="9" spans="1:23">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -3952,7 +3974,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="10" spans="1:23">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -4017,7 +4039,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="11" spans="1:23">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -4082,7 +4104,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="12" spans="1:23">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -4147,7 +4169,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="13" spans="1:23">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -4212,7 +4234,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="14" spans="1:23">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -4277,7 +4299,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="15" spans="1:23">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -4342,7 +4364,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="16" spans="1:23">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -4407,7 +4429,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="17" spans="1:23">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -4472,7 +4494,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="18" spans="1:23">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -4537,7 +4559,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="19" spans="1:23">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>39</v>
       </c>
@@ -4602,7 +4624,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="20" spans="1:23">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>40</v>
       </c>
@@ -4667,7 +4689,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="21" spans="1:23">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -4732,7 +4754,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="22" spans="1:23">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -4797,7 +4819,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="23" spans="1:23">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -4862,7 +4884,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="24" spans="1:23">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -4930,7 +4952,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="25" spans="1:23">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>45</v>
       </c>
@@ -4998,7 +5020,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="26" spans="1:23">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>46</v>
       </c>
@@ -5063,7 +5085,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="27" spans="1:23">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>47</v>
       </c>
@@ -5128,7 +5150,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="28" spans="1:23">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>48</v>
       </c>
@@ -5193,7 +5215,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="29" spans="1:23">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>49</v>
       </c>
@@ -5258,7 +5280,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="30" spans="1:23">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>50</v>
       </c>
@@ -5326,7 +5348,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="31" spans="1:23">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>51</v>
       </c>
@@ -5391,7 +5413,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="32" spans="1:23">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>52</v>
       </c>
@@ -5459,7 +5481,7 @@
         <v>879</v>
       </c>
     </row>
-    <row r="33" spans="1:23">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>53</v>
       </c>
@@ -5524,7 +5546,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="34" spans="1:23">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>54</v>
       </c>
@@ -5589,7 +5611,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="35" spans="1:23">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>55</v>
       </c>
@@ -5657,7 +5679,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="36" spans="1:23">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>56</v>
       </c>
@@ -5722,7 +5744,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="37" spans="1:23">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>57</v>
       </c>
@@ -5787,7 +5809,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="38" spans="1:23">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>58</v>
       </c>
@@ -5852,7 +5874,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="39" spans="1:23">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>59</v>
       </c>
@@ -5917,7 +5939,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="40" spans="1:23">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>60</v>
       </c>
@@ -5985,7 +6007,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="41" spans="1:23">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>61</v>
       </c>
@@ -6053,7 +6075,7 @@
         <v>882</v>
       </c>
     </row>
-    <row r="42" spans="1:23">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>62</v>
       </c>
@@ -6121,7 +6143,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="43" spans="1:23">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>63</v>
       </c>
@@ -6186,7 +6208,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="44" spans="1:23">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>64</v>
       </c>
@@ -6251,7 +6273,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="45" spans="1:23">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>65</v>
       </c>
@@ -6316,7 +6338,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="46" spans="1:23">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>66</v>
       </c>
@@ -6381,7 +6403,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="47" spans="1:23">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>67</v>
       </c>
@@ -6446,7 +6468,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="48" spans="1:23">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>68</v>
       </c>
@@ -6511,7 +6533,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="49" spans="1:23">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>69</v>
       </c>
@@ -6576,7 +6598,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="50" spans="1:23">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>70</v>
       </c>
@@ -6641,7 +6663,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="51" spans="1:23">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>71</v>
       </c>
@@ -6706,7 +6728,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="52" spans="1:23">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>72</v>
       </c>
@@ -6774,7 +6796,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="53" spans="1:23">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>73</v>
       </c>
@@ -6839,7 +6861,7 @@
         <v>853</v>
       </c>
     </row>
-    <row r="54" spans="1:23">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>74</v>
       </c>
@@ -6904,7 +6926,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="55" spans="1:23">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>75</v>
       </c>
@@ -6969,7 +6991,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="56" spans="1:23">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>76</v>
       </c>
@@ -7037,7 +7059,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="57" spans="1:23">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>77</v>
       </c>
@@ -7102,7 +7124,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="58" spans="1:23">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>78</v>
       </c>
@@ -7167,7 +7189,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="59" spans="1:23">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>79</v>
       </c>
@@ -7235,7 +7257,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="60" spans="1:23">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>80</v>
       </c>
@@ -7300,7 +7322,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="61" spans="1:23">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>81</v>
       </c>
@@ -7365,7 +7387,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="62" spans="1:23">
+    <row r="62" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>82</v>
       </c>
@@ -7430,7 +7452,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="63" spans="1:23">
+    <row r="63" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>83</v>
       </c>
@@ -7495,7 +7517,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="64" spans="1:23">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>84</v>
       </c>
@@ -7560,7 +7582,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="65" spans="1:23">
+    <row r="65" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>85</v>
       </c>
@@ -7625,7 +7647,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="66" spans="1:23">
+    <row r="66" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>86</v>
       </c>
@@ -7693,7 +7715,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="67" spans="1:23">
+    <row r="67" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>87</v>
       </c>
@@ -7758,7 +7780,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="68" spans="1:23">
+    <row r="68" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>88</v>
       </c>
@@ -7823,7 +7845,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="69" spans="1:23">
+    <row r="69" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>89</v>
       </c>
@@ -7888,7 +7910,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="70" spans="1:23">
+    <row r="70" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>90</v>
       </c>
@@ -7956,7 +7978,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="71" spans="1:23">
+    <row r="71" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>91</v>
       </c>
@@ -8021,7 +8043,7 @@
         <v>859</v>
       </c>
     </row>
-    <row r="72" spans="1:23">
+    <row r="72" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>92</v>
       </c>
@@ -8086,7 +8108,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="73" spans="1:23">
+    <row r="73" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>93</v>
       </c>
@@ -8154,7 +8176,7 @@
         <v>889</v>
       </c>
     </row>
-    <row r="74" spans="1:23">
+    <row r="74" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>94</v>
       </c>
@@ -8219,7 +8241,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="75" spans="1:23">
+    <row r="75" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>95</v>
       </c>
@@ -8287,7 +8309,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="76" spans="1:23">
+    <row r="76" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>96</v>
       </c>
@@ -8355,7 +8377,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="77" spans="1:23">
+    <row r="77" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>97</v>
       </c>
@@ -8420,7 +8442,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="78" spans="1:23">
+    <row r="78" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>98</v>
       </c>
@@ -8488,7 +8510,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="79" spans="1:23">
+    <row r="79" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>99</v>
       </c>
@@ -8556,7 +8578,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="80" spans="1:23">
+    <row r="80" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>100</v>
       </c>
@@ -8621,7 +8643,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="81" spans="1:23">
+    <row r="81" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>101</v>
       </c>
@@ -8686,7 +8708,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="82" spans="1:23">
+    <row r="82" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>102</v>
       </c>
@@ -8751,7 +8773,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="83" spans="1:23">
+    <row r="83" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>103</v>
       </c>
@@ -8816,7 +8838,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="84" spans="1:23">
+    <row r="84" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>104</v>
       </c>
@@ -8884,7 +8906,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="85" spans="1:23">
+    <row r="85" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>105</v>
       </c>
@@ -8949,7 +8971,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="86" spans="1:23">
+    <row r="86" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>106</v>
       </c>
@@ -9017,7 +9039,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="87" spans="1:23">
+    <row r="87" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>107</v>
       </c>
@@ -9082,7 +9104,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="88" spans="1:23">
+    <row r="88" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>108</v>
       </c>
@@ -9147,7 +9169,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="89" spans="1:23">
+    <row r="89" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>109</v>
       </c>
@@ -9215,7 +9237,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="90" spans="1:23">
+    <row r="90" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>110</v>
       </c>
@@ -9283,7 +9305,7 @@
         <v>897</v>
       </c>
     </row>
-    <row r="91" spans="1:23">
+    <row r="91" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>111</v>
       </c>
@@ -9351,7 +9373,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="92" spans="1:23">
+    <row r="92" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>112</v>
       </c>
@@ -9416,7 +9438,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="93" spans="1:23">
+    <row r="93" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>113</v>
       </c>
@@ -9484,7 +9506,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="94" spans="1:23">
+    <row r="94" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>114</v>
       </c>
@@ -9549,7 +9571,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="95" spans="1:23">
+    <row r="95" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>115</v>
       </c>
@@ -9617,7 +9639,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="96" spans="1:23">
+    <row r="96" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>116</v>
       </c>
@@ -9685,7 +9707,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="97" spans="1:23">
+    <row r="97" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>117</v>
       </c>
@@ -9753,7 +9775,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="98" spans="1:23">
+    <row r="98" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>118</v>
       </c>
@@ -9821,7 +9843,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="99" spans="1:23">
+    <row r="99" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>119</v>
       </c>
@@ -9886,7 +9908,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="100" spans="1:23">
+    <row r="100" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>120</v>
       </c>
@@ -9954,7 +9976,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="101" spans="1:23">
+    <row r="101" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>121</v>
       </c>
@@ -10022,7 +10044,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="102" spans="1:23">
+    <row r="102" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>122</v>
       </c>
@@ -10087,7 +10109,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="103" spans="1:23">
+    <row r="103" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>123</v>
       </c>
@@ -10152,7 +10174,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="104" spans="1:23">
+    <row r="104" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>124</v>
       </c>
@@ -10217,7 +10239,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="105" spans="1:23">
+    <row r="105" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>125</v>
       </c>
@@ -10285,7 +10307,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="106" spans="1:23">
+    <row r="106" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>126</v>
       </c>
@@ -10350,7 +10372,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="107" spans="1:23">
+    <row r="107" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>127</v>
       </c>
@@ -10415,7 +10437,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="108" spans="1:23">
+    <row r="108" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>128</v>
       </c>
@@ -10480,7 +10502,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="109" spans="1:23">
+    <row r="109" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>129</v>
       </c>
@@ -10545,7 +10567,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="110" spans="1:23">
+    <row r="110" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>130</v>
       </c>
@@ -10610,7 +10632,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="111" spans="1:23">
+    <row r="111" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>131</v>
       </c>
@@ -10678,7 +10700,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="112" spans="1:23">
+    <row r="112" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>132</v>
       </c>
@@ -10743,7 +10765,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="113" spans="1:23">
+    <row r="113" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>133</v>
       </c>
@@ -10808,7 +10830,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="114" spans="1:23">
+    <row r="114" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>134</v>
       </c>
@@ -10873,7 +10895,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="115" spans="1:23">
+    <row r="115" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>135</v>
       </c>
@@ -10938,7 +10960,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="116" spans="1:23">
+    <row r="116" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>136</v>
       </c>
@@ -11003,7 +11025,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="117" spans="1:23">
+    <row r="117" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>137</v>
       </c>
@@ -11068,7 +11090,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="118" spans="1:23">
+    <row r="118" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>138</v>
       </c>
@@ -11133,7 +11155,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="119" spans="1:23">
+    <row r="119" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>139</v>
       </c>
@@ -11198,7 +11220,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="120" spans="1:23">
+    <row r="120" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>140</v>
       </c>
@@ -11263,7 +11285,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="121" spans="1:23">
+    <row r="121" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>141</v>
       </c>
@@ -11328,7 +11350,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="122" spans="1:23">
+    <row r="122" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>142</v>
       </c>
@@ -11393,7 +11415,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="123" spans="1:23">
+    <row r="123" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>143</v>
       </c>
@@ -11458,7 +11480,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="124" spans="1:23">
+    <row r="124" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>144</v>
       </c>
@@ -11523,7 +11545,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="125" spans="1:23">
+    <row r="125" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>145</v>
       </c>
@@ -11588,7 +11610,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="126" spans="1:23">
+    <row r="126" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>146</v>
       </c>
@@ -11653,7 +11675,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="127" spans="1:23">
+    <row r="127" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>147</v>
       </c>
@@ -11721,7 +11743,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="128" spans="1:23">
+    <row r="128" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>148</v>
       </c>
@@ -11786,7 +11808,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="129" spans="1:23">
+    <row r="129" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>149</v>
       </c>
@@ -11851,7 +11873,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="130" spans="1:23">
+    <row r="130" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>150</v>
       </c>
@@ -11916,7 +11938,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="131" spans="1:23">
+    <row r="131" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>151</v>
       </c>
@@ -11981,7 +12003,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="132" spans="1:23">
+    <row r="132" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>152</v>
       </c>
@@ -12046,7 +12068,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="133" spans="1:23">
+    <row r="133" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>153</v>
       </c>
@@ -12114,7 +12136,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="134" spans="1:23">
+    <row r="134" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>154</v>
       </c>
@@ -12179,7 +12201,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="135" spans="1:23">
+    <row r="135" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>155</v>
       </c>
@@ -12244,7 +12266,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="136" spans="1:23">
+    <row r="136" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>156</v>
       </c>
@@ -12312,7 +12334,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="137" spans="1:23">
+    <row r="137" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>157</v>
       </c>
@@ -12377,7 +12399,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="138" spans="1:23">
+    <row r="138" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>158</v>
       </c>
@@ -12442,7 +12464,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="139" spans="1:23">
+    <row r="139" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>159</v>
       </c>
@@ -12510,7 +12532,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="140" spans="1:23">
+    <row r="140" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>160</v>
       </c>
@@ -12575,7 +12597,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="141" spans="1:23">
+    <row r="141" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>161</v>
       </c>
@@ -12643,7 +12665,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="142" spans="1:23">
+    <row r="142" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>162</v>
       </c>
@@ -12708,7 +12730,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="143" spans="1:23">
+    <row r="143" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>163</v>
       </c>
@@ -12776,7 +12798,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="144" spans="1:23">
+    <row r="144" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>164</v>
       </c>
@@ -12841,7 +12863,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="145" spans="1:23">
+    <row r="145" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>165</v>
       </c>
@@ -12906,7 +12928,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="146" spans="1:23">
+    <row r="146" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>166</v>
       </c>
@@ -12971,7 +12993,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="147" spans="1:23">
+    <row r="147" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>167</v>
       </c>
@@ -13036,7 +13058,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="148" spans="1:23">
+    <row r="148" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>168</v>
       </c>
@@ -13101,7 +13123,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="149" spans="1:23">
+    <row r="149" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>169</v>
       </c>
@@ -13166,7 +13188,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="150" spans="1:23">
+    <row r="150" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>170</v>
       </c>
@@ -13231,7 +13253,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="151" spans="1:23">
+    <row r="151" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>171</v>
       </c>
@@ -13299,7 +13321,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="152" spans="1:23">
+    <row r="152" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>172</v>
       </c>
@@ -13364,7 +13386,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="153" spans="1:23">
+    <row r="153" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>173</v>
       </c>
@@ -13429,7 +13451,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="154" spans="1:23">
+    <row r="154" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>174</v>
       </c>
@@ -13494,7 +13516,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="155" spans="1:23">
+    <row r="155" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>175</v>
       </c>
@@ -13559,7 +13581,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="156" spans="1:23">
+    <row r="156" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>176</v>
       </c>
@@ -13627,7 +13649,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="157" spans="1:23">
+    <row r="157" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>177</v>
       </c>
@@ -13695,7 +13717,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="158" spans="1:23">
+    <row r="158" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>178</v>
       </c>
@@ -13763,7 +13785,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="159" spans="1:23">
+    <row r="159" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>179</v>
       </c>
@@ -13831,7 +13853,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="160" spans="1:23">
+    <row r="160" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>180</v>
       </c>
@@ -13896,7 +13918,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="161" spans="1:23">
+    <row r="161" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>181</v>
       </c>
@@ -13961,7 +13983,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="162" spans="1:23">
+    <row r="162" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>182</v>
       </c>
@@ -14029,7 +14051,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="163" spans="1:23">
+    <row r="163" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>183</v>
       </c>
@@ -14094,7 +14116,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="164" spans="1:23">
+    <row r="164" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>184</v>
       </c>
@@ -14159,7 +14181,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="165" spans="1:23">
+    <row r="165" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>185</v>
       </c>
@@ -14224,7 +14246,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="166" spans="1:23">
+    <row r="166" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>186</v>
       </c>
@@ -14292,7 +14314,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="167" spans="1:23">
+    <row r="167" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>187</v>
       </c>
@@ -14360,7 +14382,7 @@
         <v>921</v>
       </c>
     </row>
-    <row r="168" spans="1:23">
+    <row r="168" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>188</v>
       </c>
@@ -14425,7 +14447,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="169" spans="1:23">
+    <row r="169" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>189</v>
       </c>
@@ -14490,7 +14512,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="170" spans="1:23">
+    <row r="170" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>190</v>
       </c>
@@ -14555,7 +14577,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="171" spans="1:23">
+    <row r="171" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>191</v>
       </c>
@@ -14620,7 +14642,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="172" spans="1:23">
+    <row r="172" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>192</v>
       </c>
@@ -14685,7 +14707,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="173" spans="1:23">
+    <row r="173" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>193</v>
       </c>
@@ -14750,7 +14772,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="174" spans="1:23">
+    <row r="174" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>194</v>
       </c>
@@ -14818,7 +14840,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="175" spans="1:23">
+    <row r="175" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>195</v>
       </c>
@@ -14883,7 +14905,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="176" spans="1:23">
+    <row r="176" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>196</v>
       </c>
@@ -14948,7 +14970,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="177" spans="1:23">
+    <row r="177" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>197</v>
       </c>
@@ -15013,7 +15035,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="178" spans="1:23">
+    <row r="178" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>198</v>
       </c>
@@ -15078,7 +15100,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="179" spans="1:23">
+    <row r="179" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>199</v>
       </c>
@@ -15143,7 +15165,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="180" spans="1:23">
+    <row r="180" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>200</v>
       </c>
@@ -15208,7 +15230,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="181" spans="1:23">
+    <row r="181" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>201</v>
       </c>
@@ -15273,7 +15295,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="182" spans="1:23">
+    <row r="182" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>202</v>
       </c>
@@ -15338,7 +15360,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="183" spans="1:23">
+    <row r="183" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>203</v>
       </c>
@@ -15403,7 +15425,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="184" spans="1:23">
+    <row r="184" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>204</v>
       </c>
@@ -15468,7 +15490,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="185" spans="1:23">
+    <row r="185" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>205</v>
       </c>
@@ -15533,7 +15555,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="186" spans="1:23">
+    <row r="186" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>206</v>
       </c>
@@ -15598,7 +15620,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="187" spans="1:23">
+    <row r="187" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>207</v>
       </c>
@@ -15663,7 +15685,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="188" spans="1:23">
+    <row r="188" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>208</v>
       </c>
@@ -15728,7 +15750,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="189" spans="1:23">
+    <row r="189" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>209</v>
       </c>
@@ -15796,7 +15818,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="190" spans="1:23">
+    <row r="190" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>210</v>
       </c>
@@ -15861,7 +15883,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="191" spans="1:23">
+    <row r="191" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>211</v>
       </c>
@@ -15926,7 +15948,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="192" spans="1:23">
+    <row r="192" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>212</v>
       </c>
@@ -15994,7 +16016,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="193" spans="1:23">
+    <row r="193" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>213</v>
       </c>
@@ -16059,7 +16081,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="194" spans="1:23">
+    <row r="194" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>214</v>
       </c>
@@ -16124,7 +16146,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="195" spans="1:23">
+    <row r="195" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>215</v>
       </c>
@@ -16189,7 +16211,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="196" spans="1:23">
+    <row r="196" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>216</v>
       </c>
@@ -16257,7 +16279,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="197" spans="1:23">
+    <row r="197" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>217</v>
       </c>
@@ -16322,7 +16344,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="198" spans="1:23">
+    <row r="198" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>218</v>
       </c>
@@ -16387,7 +16409,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="199" spans="1:23">
+    <row r="199" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>219</v>
       </c>
@@ -16452,7 +16474,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="200" spans="1:23">
+    <row r="200" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>220</v>
       </c>
@@ -16520,7 +16542,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="201" spans="1:23">
+    <row r="201" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>221</v>
       </c>
@@ -16588,7 +16610,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="202" spans="1:23">
+    <row r="202" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>222</v>
       </c>
@@ -16653,7 +16675,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="203" spans="1:23">
+    <row r="203" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>223</v>
       </c>
@@ -16721,7 +16743,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="204" spans="1:23">
+    <row r="204" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>224</v>
       </c>
@@ -16786,7 +16808,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="205" spans="1:23">
+    <row r="205" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>225</v>
       </c>
@@ -16851,7 +16873,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="206" spans="1:23">
+    <row r="206" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>226</v>
       </c>
@@ -16919,7 +16941,7 @@
         <v>929</v>
       </c>
     </row>
-    <row r="207" spans="1:23">
+    <row r="207" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>227</v>
       </c>
@@ -16984,7 +17006,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="208" spans="1:23">
+    <row r="208" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>228</v>
       </c>
@@ -17049,7 +17071,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="209" spans="1:23">
+    <row r="209" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>229</v>
       </c>
@@ -17117,7 +17139,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="210" spans="1:23">
+    <row r="210" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>230</v>
       </c>
@@ -17185,7 +17207,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="211" spans="1:23">
+    <row r="211" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>231</v>
       </c>
@@ -17253,7 +17275,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="212" spans="1:23">
+    <row r="212" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>232</v>
       </c>
@@ -17318,7 +17340,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="213" spans="1:23">
+    <row r="213" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>233</v>
       </c>
@@ -17383,7 +17405,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="214" spans="1:23">
+    <row r="214" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>234</v>
       </c>
@@ -17448,7 +17470,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="215" spans="1:23">
+    <row r="215" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>235</v>
       </c>
@@ -17513,7 +17535,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="216" spans="1:23">
+    <row r="216" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>236</v>
       </c>
@@ -17581,7 +17603,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="217" spans="1:23">
+    <row r="217" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>237</v>
       </c>
@@ -17646,7 +17668,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="218" spans="1:23">
+    <row r="218" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>238</v>
       </c>
@@ -17714,7 +17736,7 @@
         <v>934</v>
       </c>
     </row>
-    <row r="219" spans="1:23">
+    <row r="219" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>239</v>
       </c>
@@ -17779,7 +17801,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="220" spans="1:23">
+    <row r="220" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>240</v>
       </c>
@@ -17847,7 +17869,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="221" spans="1:23">
+    <row r="221" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>241</v>
       </c>
@@ -17912,7 +17934,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="222" spans="1:23">
+    <row r="222" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>242</v>
       </c>
@@ -17980,7 +18002,7 @@
         <v>936</v>
       </c>
     </row>
-    <row r="223" spans="1:23">
+    <row r="223" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>243</v>
       </c>
@@ -18045,7 +18067,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="224" spans="1:23">
+    <row r="224" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>244</v>
       </c>
@@ -18110,7 +18132,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="225" spans="1:23">
+    <row r="225" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>245</v>
       </c>
@@ -18178,7 +18200,7 @@
         <v>937</v>
       </c>
     </row>
-    <row r="226" spans="1:23">
+    <row r="226" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>246</v>
       </c>
@@ -18243,7 +18265,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="227" spans="1:23">
+    <row r="227" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>247</v>
       </c>
@@ -18308,7 +18330,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="228" spans="1:23">
+    <row r="228" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>248</v>
       </c>
@@ -18376,7 +18398,7 @@
         <v>938</v>
       </c>
     </row>
-    <row r="229" spans="1:23">
+    <row r="229" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>249</v>
       </c>
@@ -18444,7 +18466,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="230" spans="1:23">
+    <row r="230" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>250</v>
       </c>
@@ -18512,7 +18534,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="231" spans="1:23">
+    <row r="231" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>251</v>
       </c>
@@ -18580,7 +18602,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="232" spans="1:23">
+    <row r="232" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>252</v>
       </c>
@@ -18648,7 +18670,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="233" spans="1:23">
+    <row r="233" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>253</v>
       </c>
@@ -18716,7 +18738,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="234" spans="1:23">
+    <row r="234" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>254</v>
       </c>
@@ -18784,7 +18806,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="235" spans="1:23">
+    <row r="235" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>255</v>
       </c>
@@ -18852,7 +18874,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="236" spans="1:23">
+    <row r="236" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>256</v>
       </c>
@@ -18920,7 +18942,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="237" spans="1:23">
+    <row r="237" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>257</v>
       </c>
@@ -18988,7 +19010,7 @@
         <v>947</v>
       </c>
     </row>
-    <row r="238" spans="1:23">
+    <row r="238" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>258</v>
       </c>
@@ -19056,7 +19078,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="239" spans="1:23">
+    <row r="239" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>259</v>
       </c>
@@ -19121,7 +19143,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="240" spans="1:23">
+    <row r="240" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>260</v>
       </c>
@@ -19189,7 +19211,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="241" spans="1:23">
+    <row r="241" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>261</v>
       </c>
@@ -19257,7 +19279,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="242" spans="1:23">
+    <row r="242" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>262</v>
       </c>
@@ -19325,7 +19347,7 @@
         <v>951</v>
       </c>
     </row>
-    <row r="243" spans="1:23">
+    <row r="243" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>263</v>
       </c>
@@ -19393,7 +19415,7 @@
         <v>951</v>
       </c>
     </row>
-    <row r="244" spans="1:23">
+    <row r="244" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>264</v>
       </c>
@@ -19458,7 +19480,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="245" spans="1:23">
+    <row r="245" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>265</v>
       </c>
@@ -19523,7 +19545,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="246" spans="1:23">
+    <row r="246" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>266</v>
       </c>
@@ -19591,7 +19613,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="247" spans="1:23">
+    <row r="247" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>267</v>
       </c>
@@ -19656,7 +19678,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="248" spans="1:23">
+    <row r="248" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>268</v>
       </c>
@@ -19724,7 +19746,7 @@
         <v>953</v>
       </c>
     </row>
-    <row r="249" spans="1:23">
+    <row r="249" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>269</v>
       </c>
@@ -19792,7 +19814,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="250" spans="1:23">
+    <row r="250" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>270</v>
       </c>
@@ -19860,7 +19882,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="251" spans="1:23">
+    <row r="251" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>271</v>
       </c>
@@ -19925,7 +19947,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="252" spans="1:23">
+    <row r="252" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>272</v>
       </c>
@@ -19990,7 +20012,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="253" spans="1:23">
+    <row r="253" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>273</v>
       </c>
@@ -20055,7 +20077,7 @@
         <v>853</v>
       </c>
     </row>
-    <row r="254" spans="1:23">
+    <row r="254" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>274</v>
       </c>
@@ -20120,7 +20142,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="255" spans="1:23">
+    <row r="255" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>275</v>
       </c>
@@ -20185,7 +20207,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="256" spans="1:23">
+    <row r="256" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>276</v>
       </c>
@@ -20250,7 +20272,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="257" spans="1:23">
+    <row r="257" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>277</v>
       </c>
@@ -20318,7 +20340,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="258" spans="1:23">
+    <row r="258" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>278</v>
       </c>
@@ -20386,7 +20408,7 @@
         <v>957</v>
       </c>
     </row>
-    <row r="259" spans="1:23">
+    <row r="259" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>279</v>
       </c>
@@ -20451,7 +20473,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="260" spans="1:23">
+    <row r="260" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>280</v>
       </c>
@@ -20516,7 +20538,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="261" spans="1:23">
+    <row r="261" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>281</v>
       </c>
@@ -20581,7 +20603,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="262" spans="1:23">
+    <row r="262" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>282</v>
       </c>
@@ -20646,7 +20668,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="263" spans="1:23">
+    <row r="263" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>283</v>
       </c>
@@ -20711,7 +20733,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="264" spans="1:23">
+    <row r="264" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>284</v>
       </c>
@@ -20779,7 +20801,7 @@
         <v>958</v>
       </c>
     </row>
-    <row r="265" spans="1:23">
+    <row r="265" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>285</v>
       </c>
@@ -20844,7 +20866,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="266" spans="1:23">
+    <row r="266" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>286</v>
       </c>
@@ -20909,7 +20931,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="267" spans="1:23">
+    <row r="267" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>287</v>
       </c>
@@ -20974,7 +20996,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="268" spans="1:23">
+    <row r="268" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>288</v>
       </c>
@@ -21042,7 +21064,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="269" spans="1:23">
+    <row r="269" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>289</v>
       </c>
@@ -21110,7 +21132,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="270" spans="1:23">
+    <row r="270" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>290</v>
       </c>
@@ -21178,7 +21200,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="271" spans="1:23">
+    <row r="271" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>291</v>
       </c>
@@ -21246,7 +21268,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="272" spans="1:23">
+    <row r="272" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>292</v>
       </c>
@@ -21311,7 +21333,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="273" spans="1:23">
+    <row r="273" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>293</v>
       </c>
@@ -21376,7 +21398,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="274" spans="1:23">
+    <row r="274" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>294</v>
       </c>
@@ -21444,7 +21466,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="275" spans="1:23">
+    <row r="275" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>295</v>
       </c>
@@ -21509,7 +21531,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="276" spans="1:23">
+    <row r="276" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>296</v>
       </c>
@@ -21577,7 +21599,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="277" spans="1:23">
+    <row r="277" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>297</v>
       </c>
@@ -21645,7 +21667,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="278" spans="1:23">
+    <row r="278" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>298</v>
       </c>
@@ -21713,7 +21735,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="279" spans="1:23">
+    <row r="279" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>299</v>
       </c>
@@ -21781,7 +21803,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="280" spans="1:23">
+    <row r="280" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>300</v>
       </c>
@@ -21849,7 +21871,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="281" spans="1:23">
+    <row r="281" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>301</v>
       </c>
@@ -21914,7 +21936,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="282" spans="1:23">
+    <row r="282" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>302</v>
       </c>
@@ -21982,7 +22004,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="283" spans="1:23">
+    <row r="283" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>303</v>
       </c>
@@ -22047,7 +22069,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="284" spans="1:23">
+    <row r="284" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>304</v>
       </c>
@@ -22115,7 +22137,7 @@
         <v>969</v>
       </c>
     </row>
-    <row r="285" spans="1:23">
+    <row r="285" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>305</v>
       </c>
@@ -22180,7 +22202,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="286" spans="1:23">
+    <row r="286" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
         <v>306</v>
       </c>
@@ -22248,7 +22270,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="287" spans="1:23">
+    <row r="287" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>307</v>
       </c>
@@ -22313,7 +22335,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="288" spans="1:23">
+    <row r="288" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>308</v>
       </c>
@@ -22381,7 +22403,7 @@
         <v>971</v>
       </c>
     </row>
-    <row r="289" spans="1:23">
+    <row r="289" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>309</v>
       </c>
@@ -22449,7 +22471,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="290" spans="1:23">
+    <row r="290" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>310</v>
       </c>
@@ -22508,7 +22530,7 @@
         <v>973</v>
       </c>
     </row>
-    <row r="291" spans="1:23">
+    <row r="291" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>311</v>
       </c>
@@ -22564,7 +22586,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="292" spans="1:23">
+    <row r="292" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>312</v>
       </c>
@@ -22622,104 +22644,104 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="W24" r:id="rId1"/>
-    <hyperlink ref="W25" r:id="rId2"/>
-    <hyperlink ref="W30" r:id="rId3"/>
-    <hyperlink ref="W32" r:id="rId4"/>
-    <hyperlink ref="W35" r:id="rId5"/>
-    <hyperlink ref="W40" r:id="rId6"/>
-    <hyperlink ref="W41" r:id="rId7"/>
-    <hyperlink ref="W42" r:id="rId8"/>
-    <hyperlink ref="W52" r:id="rId9"/>
-    <hyperlink ref="W56" r:id="rId10"/>
-    <hyperlink ref="W59" r:id="rId11"/>
-    <hyperlink ref="W66" r:id="rId12"/>
-    <hyperlink ref="W70" r:id="rId13"/>
-    <hyperlink ref="W73" r:id="rId14"/>
-    <hyperlink ref="W75" r:id="rId15"/>
-    <hyperlink ref="W76" r:id="rId16"/>
-    <hyperlink ref="W78" r:id="rId17"/>
-    <hyperlink ref="W79" r:id="rId18"/>
-    <hyperlink ref="W84" r:id="rId19"/>
-    <hyperlink ref="W86" r:id="rId20"/>
-    <hyperlink ref="W89" r:id="rId21"/>
-    <hyperlink ref="W90" r:id="rId22"/>
-    <hyperlink ref="W91" r:id="rId23"/>
-    <hyperlink ref="W93" r:id="rId24"/>
-    <hyperlink ref="W95" r:id="rId25"/>
-    <hyperlink ref="W96" r:id="rId26"/>
-    <hyperlink ref="W97" r:id="rId27"/>
-    <hyperlink ref="W98" r:id="rId28"/>
-    <hyperlink ref="W100" r:id="rId29"/>
-    <hyperlink ref="W105" r:id="rId30"/>
-    <hyperlink ref="W111" r:id="rId31"/>
-    <hyperlink ref="W127" r:id="rId32"/>
-    <hyperlink ref="W133" r:id="rId33"/>
-    <hyperlink ref="W136" r:id="rId34"/>
-    <hyperlink ref="W139" r:id="rId35"/>
-    <hyperlink ref="W141" r:id="rId36"/>
-    <hyperlink ref="W143" r:id="rId37"/>
-    <hyperlink ref="W151" r:id="rId38"/>
-    <hyperlink ref="W156" r:id="rId39"/>
-    <hyperlink ref="W157" r:id="rId40"/>
-    <hyperlink ref="W158" r:id="rId41"/>
-    <hyperlink ref="W159" r:id="rId42"/>
-    <hyperlink ref="W162" r:id="rId43"/>
-    <hyperlink ref="W166" r:id="rId44"/>
-    <hyperlink ref="W167" r:id="rId45"/>
-    <hyperlink ref="W174" r:id="rId46"/>
-    <hyperlink ref="W189" r:id="rId47"/>
-    <hyperlink ref="W192" r:id="rId48"/>
-    <hyperlink ref="W196" r:id="rId49"/>
-    <hyperlink ref="W200" r:id="rId50"/>
-    <hyperlink ref="W201" r:id="rId51"/>
-    <hyperlink ref="W203" r:id="rId52"/>
-    <hyperlink ref="W206" r:id="rId53"/>
-    <hyperlink ref="W209" r:id="rId54"/>
-    <hyperlink ref="W210" r:id="rId55"/>
-    <hyperlink ref="W211" r:id="rId56"/>
-    <hyperlink ref="W216" r:id="rId57"/>
-    <hyperlink ref="W218" r:id="rId58"/>
-    <hyperlink ref="W220" r:id="rId59"/>
-    <hyperlink ref="W222" r:id="rId60" location="zoom=50&#10;https://www.accenture.com/gb-en/services/data-ai/responsible-ai?form=MG0AV3"/>
-    <hyperlink ref="W225" r:id="rId61"/>
-    <hyperlink ref="W228" r:id="rId62"/>
-    <hyperlink ref="W229" r:id="rId63"/>
-    <hyperlink ref="W230" r:id="rId64"/>
-    <hyperlink ref="W231" r:id="rId65"/>
-    <hyperlink ref="W232" r:id="rId66"/>
-    <hyperlink ref="W233" r:id="rId67"/>
-    <hyperlink ref="W234" r:id="rId68"/>
-    <hyperlink ref="W235" r:id="rId69"/>
-    <hyperlink ref="W236" r:id="rId70"/>
-    <hyperlink ref="W237" r:id="rId71"/>
-    <hyperlink ref="W238" r:id="rId72"/>
-    <hyperlink ref="W240" r:id="rId73"/>
-    <hyperlink ref="W241" r:id="rId74"/>
-    <hyperlink ref="W242" r:id="rId75"/>
-    <hyperlink ref="W243" r:id="rId76"/>
-    <hyperlink ref="W246" r:id="rId77"/>
-    <hyperlink ref="W249" r:id="rId78"/>
-    <hyperlink ref="W250" r:id="rId79"/>
-    <hyperlink ref="W257" r:id="rId80"/>
-    <hyperlink ref="W258" r:id="rId81"/>
-    <hyperlink ref="W264" r:id="rId82"/>
-    <hyperlink ref="W268" r:id="rId83"/>
-    <hyperlink ref="W269" r:id="rId84"/>
-    <hyperlink ref="W270" r:id="rId85"/>
-    <hyperlink ref="W271" r:id="rId86"/>
-    <hyperlink ref="W274" r:id="rId87"/>
-    <hyperlink ref="W276" r:id="rId88"/>
-    <hyperlink ref="W277" r:id="rId89"/>
-    <hyperlink ref="W278" r:id="rId90"/>
-    <hyperlink ref="W279" r:id="rId91"/>
-    <hyperlink ref="W280" r:id="rId92"/>
-    <hyperlink ref="W282" r:id="rId93"/>
-    <hyperlink ref="W284" r:id="rId94"/>
-    <hyperlink ref="W286" r:id="rId95"/>
-    <hyperlink ref="W288" r:id="rId96"/>
-    <hyperlink ref="W289" r:id="rId97"/>
-    <hyperlink ref="W290" r:id="rId98"/>
+    <hyperlink ref="W24" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="W25" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="W30" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="W32" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="W35" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="W40" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="W41" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="W42" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="W52" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="W56" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="W59" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="W66" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="W70" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="W73" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="W75" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="W76" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="W78" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="W79" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="W84" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="W86" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="W89" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="W90" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="W91" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="W93" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="W95" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="W96" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="W97" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="W98" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="W100" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="W105" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="W111" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="W127" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="W133" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="W136" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="W139" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="W141" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="W143" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="W151" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="W156" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="W157" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="W158" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="W159" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="W162" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="W166" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="W167" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="W174" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="W189" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="W192" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="W196" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="W200" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="W201" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="W203" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="W206" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="W209" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="W210" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="W211" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="W216" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="W218" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="W220" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="W222" r:id="rId60" location="zoom=50_x000a_https://www.accenture.com/gb-en/services/data-ai/responsible-ai?form=MG0AV3" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="W225" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="W228" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="W229" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="W230" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="W231" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="W232" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="W233" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="W234" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="W235" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="W236" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="W237" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="W238" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="W240" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="W241" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="W242" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="W243" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="W246" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="W249" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="W250" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="W257" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="W258" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="W264" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="W268" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="W269" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="W270" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="W271" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="W274" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="W276" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="W277" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="W278" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="W279" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="W280" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="W282" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="W284" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="W286" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="W288" r:id="rId96" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="W289" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="W290" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>